<commit_message>
Developed and executed  Tc's 12207 and 12209
</commit_message>
<xml_diff>
--- a/TestData/DPPTestData.xlsx
+++ b/TestData/DPPTestData.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D22A3200-1812-4EA7-B350-FD1EBCFC0B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19635" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Payments" sheetId="1" r:id="rId1"/>
+    <sheet name="Payments2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="97">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -232,52 +216,475 @@
   </si>
   <si>
     <t>dinersclub</t>
+  </si>
+  <si>
+    <t>StateCode</t>
+  </si>
+  <si>
+    <t>SaleItemQuantity</t>
+  </si>
+  <si>
+    <t>AmountTendered</t>
+  </si>
+  <si>
+    <t>QuickSaleItemNameTwo</t>
+  </si>
+  <si>
+    <t>QuickSaleItemPriceTwo</t>
+  </si>
+  <si>
+    <t>QuickSaleItemTaxTwo</t>
+  </si>
+  <si>
+    <t>AccountNickName</t>
+  </si>
+  <si>
+    <t>RoutingNumber</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>RecurringStatus</t>
+  </si>
+  <si>
+    <t>PaymentStatus</t>
+  </si>
+  <si>
+    <t>MID</t>
+  </si>
+  <si>
+    <t>SearchTransactionField</t>
+  </si>
+  <si>
+    <t>ShippingMethod</t>
+  </si>
+  <si>
+    <t>TC_12206</t>
+  </si>
+  <si>
+    <t>Credit/Refund</t>
+  </si>
+  <si>
+    <t>IATS ZENTRO</t>
+  </si>
+  <si>
+    <t>avins</t>
+  </si>
+  <si>
+    <t>god</t>
+  </si>
+  <si>
+    <t>Testcust@gmail.com</t>
+  </si>
+  <si>
+    <t>ACH/EFT</t>
+  </si>
+  <si>
+    <t>12st Main Road</t>
+  </si>
+  <si>
+    <t>New Holland</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Buy Product</t>
+  </si>
+  <si>
+    <t>ACH Account</t>
+  </si>
+  <si>
+    <t>Checking</t>
+  </si>
+  <si>
+    <t>TC_12208</t>
+  </si>
+  <si>
+    <t>avinsgod@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -285,30 +692,318 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -357,7 +1052,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -390,26 +1085,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -442,23 +1120,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -600,38 +1261,33 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="19.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="11" max="11" width="18.8571428571429" customWidth="1"/>
+    <col min="14" max="14" width="19.2857142857143" customWidth="1"/>
     <col min="15" max="15" width="24" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" customWidth="1"/>
-    <col min="18" max="20" width="16.42578125" customWidth="1"/>
-    <col min="21" max="22" width="17.28515625" customWidth="1"/>
-    <col min="32" max="32" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="17.4285714285714" customWidth="1"/>
+    <col min="17" max="17" width="21.4285714285714" customWidth="1"/>
+    <col min="18" max="20" width="16.4285714285714" customWidth="1"/>
+    <col min="21" max="22" width="17.2857142857143" customWidth="1"/>
+    <col min="32" max="32" width="14.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -695,10 +1351,10 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="W1" t="s">
@@ -738,7 +1394,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -751,7 +1407,7 @@
       <c r="E2">
         <v>50</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I2">
@@ -760,7 +1416,7 @@
       <c r="J2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="9" t="s">
         <v>39</v>
       </c>
       <c r="L2">
@@ -828,7 +1484,7 @@
       <c r="G3" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I3">
@@ -837,7 +1493,7 @@
       <c r="J3" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="10" t="s">
         <v>39</v>
       </c>
       <c r="L3">
@@ -870,10 +1526,10 @@
       <c r="AF3" t="b">
         <v>0</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AG3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AH3" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -890,7 +1546,7 @@
       <c r="E4">
         <v>50</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I4">
@@ -899,7 +1555,7 @@
       <c r="J4" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="9" t="s">
         <v>54</v>
       </c>
       <c r="L4">
@@ -947,10 +1603,10 @@
       <c r="AF4" t="b">
         <v>0</v>
       </c>
-      <c r="AG4" s="2" t="s">
+      <c r="AG4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AH4" s="2" t="s">
+      <c r="AH4" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -967,7 +1623,7 @@
       <c r="E5">
         <v>55</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I5">
@@ -976,7 +1632,7 @@
       <c r="J5" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="9" t="s">
         <v>58</v>
       </c>
       <c r="L5">
@@ -1027,10 +1683,10 @@
       <c r="AF5" t="b">
         <v>1</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AG5" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AH5" s="2" t="s">
+      <c r="AH5" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1047,7 +1703,7 @@
       <c r="E6">
         <v>55</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I6">
@@ -1056,7 +1712,7 @@
       <c r="J6" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="9" t="s">
         <v>62</v>
       </c>
       <c r="L6">
@@ -1113,10 +1769,10 @@
       <c r="AF6" t="b">
         <v>1</v>
       </c>
-      <c r="AG6" s="2" t="s">
+      <c r="AG6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AH6" s="2" t="s">
+      <c r="AH6" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1133,7 +1789,7 @@
       <c r="E7">
         <v>35</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="6" t="s">
         <v>37</v>
       </c>
       <c r="I7">
@@ -1142,7 +1798,7 @@
       <c r="J7" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="9" t="s">
         <v>65</v>
       </c>
       <c r="L7">
@@ -1184,30 +1840,310 @@
       <c r="AF7" t="b">
         <v>1</v>
       </c>
-      <c r="AG7" s="2" t="s">
+      <c r="AG7" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AH7" s="2" t="s">
+      <c r="AH7" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
-      <c r="AG8" s="2" t="s">
+    <row r="8" spans="33:34">
+      <c r="AG8" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AH8" s="2" t="s">
+      <c r="AH8" s="9" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{A1451763-5D6F-4816-AA0A-B3215E232D9F}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{D1428BDC-B790-455D-BBC1-37B923268189}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{0FF48CAA-353C-44EC-B49A-48B3FDB691C9}"/>
-    <hyperlink ref="H6" r:id="rId4" xr:uid="{407A9E7C-3F14-4AD8-BB85-C4BCBA63E87B}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{E10D4276-F3E1-4124-B1E5-422134A1F8F2}"/>
-    <hyperlink ref="H3" r:id="rId6" xr:uid="{1FCC6AFE-A186-42D8-BF07-6E3C73DC6AA9}"/>
+    <hyperlink ref="H4" r:id="rId1" display="test@gmail.com"/>
+    <hyperlink ref="H2" r:id="rId1" display="test@gmail.com"/>
+    <hyperlink ref="H5" r:id="rId1" display="test@gmail.com"/>
+    <hyperlink ref="H6" r:id="rId1" display="test@gmail.com"/>
+    <hyperlink ref="H7" r:id="rId1" display="test@gmail.com"/>
+    <hyperlink ref="H3" r:id="rId1" display="test@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AQ3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="21.7142857142857" defaultRowHeight="15" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="16384" width="21.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:43">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:38">
+      <c r="A2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1231233332</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" s="2">
+        <v>17557</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>123123123</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:29">
+      <c r="A3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1231233332</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="1">
+        <v>43567</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="Testcust@gmail.com"/>
+    <hyperlink ref="H3" r:id="rId2" display="avinsgod@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created 11043 and 11044
</commit_message>
<xml_diff>
--- a/TestData/DPPTestData.xlsx
+++ b/TestData/DPPTestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27511"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D22A3200-1812-4EA7-B350-FD1EBCFC0B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9FF9591-AD7A-4469-8E2C-8554B4A3269D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="75">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -232,13 +232,37 @@
   </si>
   <si>
     <t>dinersclub</t>
+  </si>
+  <si>
+    <t>TC_11043</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>amextest@gmail.com</t>
+  </si>
+  <si>
+    <t>0832</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>12stMainRoad</t>
+  </si>
+  <si>
+    <t>NewHolland</t>
+  </si>
+  <si>
+    <t>Buy Product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +292,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -290,12 +319,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -613,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1192,6 +1224,85 @@
       </c>
     </row>
     <row r="8" spans="1:34">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="5">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1231233332</v>
+      </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="6">
+        <v>378282246310005</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" t="s">
+        <v>43</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>17557</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE8">
+        <v>12345</v>
+      </c>
+      <c r="AF8" t="b">
+        <v>1</v>
+      </c>
       <c r="AG8" s="2" t="s">
         <v>52</v>
       </c>
@@ -1207,6 +1318,7 @@
     <hyperlink ref="H6" r:id="rId4" xr:uid="{407A9E7C-3F14-4AD8-BB85-C4BCBA63E87B}"/>
     <hyperlink ref="H7" r:id="rId5" xr:uid="{E10D4276-F3E1-4124-B1E5-422134A1F8F2}"/>
     <hyperlink ref="H3" r:id="rId6" xr:uid="{1FCC6AFE-A186-42D8-BF07-6E3C73DC6AA9}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{1A10BA7E-B5CD-4694-A3B3-BDFDF3B6FD34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TC_12207 and 12209 and 11007 test cases executions are completed
</commit_message>
<xml_diff>
--- a/TestData/DPPTestData.xlsx
+++ b/TestData/DPPTestData.xlsx
@@ -1874,8 +1874,8 @@
   <sheetPr/>
   <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7142857142857" defaultRowHeight="15" outlineLevelRow="2"/>

</xml_diff>